<commit_message>
Everything works now: Updated Requirement excel sheets for all locations to hold 5 requirements instead of 3. Also, multiple exceptions are handled properly now
</commit_message>
<xml_diff>
--- a/Convos/Shifts.xlsx
+++ b/Convos/Shifts.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="45" windowWidth="18195" windowHeight="7995" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="612" windowWidth="23256" windowHeight="11736" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Call Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="145621" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -70,11 +70,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,22 +445,20 @@
   <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="topLeft" state="frozen"/>
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="2.786830357142857" customWidth="1" min="1" max="1"/>
-    <col width="1.358258928571429" customWidth="1" min="2" max="2"/>
-    <col width="0.7868303571428571" customWidth="1" min="3" max="3"/>
-    <col width="0.7868303571428571" customWidth="1" min="4" max="4"/>
-    <col width="9.714285714285714" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="13.71428571428571" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="26.71428571428572" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="0.6439732142857143" customWidth="1" min="8" max="8"/>
-    <col width="0.6439732142857143" customWidth="1" min="9" max="9"/>
-    <col width="30.71428571428572" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="2.77734375" customWidth="1" style="5" min="1" max="1"/>
+    <col width="1.33203125" customWidth="1" style="5" min="2" max="2"/>
+    <col width="0.77734375" customWidth="1" style="5" min="3" max="4"/>
+    <col width="9.6640625" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.6640625" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="26.6640625" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
+    <col width="0.6640625" customWidth="1" style="5" min="8" max="9"/>
+    <col width="30.6640625" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -510,14 +510,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Employee: Acton, Hannah</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n"/>
+      <c r="A3" s="4" t="n"/>
       <c r="B3" s="3" t="n">
         <v>45572</v>
       </c>
@@ -550,7 +550,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
+      <c r="A4" s="4" t="n"/>
       <c r="B4" s="3" t="n">
         <v>45573</v>
       </c>
@@ -578,7 +578,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
+      <c r="A5" s="4" t="n"/>
       <c r="B5" s="3" t="n">
         <v>45575</v>
       </c>
@@ -606,7 +606,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n"/>
+      <c r="A6" s="4" t="n"/>
       <c r="B6" s="3" t="n">
         <v>45576</v>
       </c>
@@ -634,34 +634,34 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="4" t="n"/>
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="4" t="n"/>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t>Count: 4</t>
         </is>
       </c>
-      <c r="G7" s="2" t="n"/>
-      <c r="H7" s="2" t="inlineStr">
+      <c r="G7" s="4" t="n"/>
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>13.50</t>
         </is>
       </c>
-      <c r="I7" s="2" t="inlineStr"/>
-      <c r="J7" s="2" t="n"/>
+      <c r="I7" s="4" t="n"/>
+      <c r="J7" s="4" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Employee: Anderson, Gracie</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n"/>
+      <c r="A9" s="4" t="n"/>
       <c r="B9" s="3" t="n">
         <v>45572</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
+      <c r="A10" s="4" t="n"/>
       <c r="B10" s="3" t="n">
         <v>45572</v>
       </c>
@@ -722,7 +722,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n"/>
+      <c r="A11" s="4" t="n"/>
       <c r="B11" s="3" t="n">
         <v>45573</v>
       </c>
@@ -755,7 +755,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n"/>
+      <c r="A12" s="4" t="n"/>
       <c r="B12" s="3" t="n">
         <v>45575</v>
       </c>
@@ -788,7 +788,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n"/>
+      <c r="A13" s="4" t="n"/>
       <c r="B13" s="3" t="n">
         <v>45576</v>
       </c>
@@ -816,34 +816,34 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
-      <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
-      <c r="E14" s="2" t="n"/>
-      <c r="F14" s="2" t="inlineStr">
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="4" t="n"/>
+      <c r="C14" s="4" t="n"/>
+      <c r="D14" s="4" t="n"/>
+      <c r="E14" s="4" t="n"/>
+      <c r="F14" s="4" t="inlineStr">
         <is>
           <t>Count: 5</t>
         </is>
       </c>
-      <c r="G14" s="2" t="n"/>
-      <c r="H14" s="2" t="inlineStr">
+      <c r="G14" s="4" t="n"/>
+      <c r="H14" s="4" t="inlineStr">
         <is>
           <t>19.00</t>
         </is>
       </c>
-      <c r="I14" s="2" t="inlineStr"/>
-      <c r="J14" s="2" t="n"/>
+      <c r="I14" s="4" t="n"/>
+      <c r="J14" s="4" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="A15" s="4" t="inlineStr">
         <is>
           <t>Employee: Baumer, Kasey</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n"/>
+      <c r="A16" s="4" t="n"/>
       <c r="B16" s="3" t="n">
         <v>45571</v>
       </c>
@@ -871,7 +871,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n"/>
+      <c r="A17" s="4" t="n"/>
       <c r="B17" s="3" t="n">
         <v>45572</v>
       </c>
@@ -899,7 +899,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n"/>
+      <c r="A18" s="4" t="n"/>
       <c r="B18" s="3" t="n">
         <v>45576</v>
       </c>
@@ -932,34 +932,34 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
-      <c r="C19" s="2" t="n"/>
-      <c r="D19" s="2" t="n"/>
-      <c r="E19" s="2" t="n"/>
-      <c r="F19" s="2" t="inlineStr">
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="4" t="n"/>
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="4" t="n"/>
+      <c r="E19" s="4" t="n"/>
+      <c r="F19" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G19" s="2" t="n"/>
-      <c r="H19" s="2" t="inlineStr">
+      <c r="G19" s="4" t="n"/>
+      <c r="H19" s="4" t="inlineStr">
         <is>
           <t>9.00</t>
         </is>
       </c>
-      <c r="I19" s="2" t="inlineStr"/>
-      <c r="J19" s="2" t="n"/>
+      <c r="I19" s="4" t="n"/>
+      <c r="J19" s="4" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="inlineStr">
+      <c r="A20" s="4" t="inlineStr">
         <is>
           <t>Employee: Blackburn, Logan</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="n"/>
+      <c r="A21" s="4" t="n"/>
       <c r="B21" s="3" t="n">
         <v>45571</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n"/>
+      <c r="A22" s="4" t="n"/>
       <c r="B22" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1020,7 +1020,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="n"/>
+      <c r="A23" s="4" t="n"/>
       <c r="B23" s="3" t="n">
         <v>45574</v>
       </c>
@@ -1053,7 +1053,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n"/>
+      <c r="A24" s="4" t="n"/>
       <c r="B24" s="3" t="n">
         <v>45575</v>
       </c>
@@ -1091,34 +1091,34 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n"/>
-      <c r="B25" s="2" t="n"/>
-      <c r="C25" s="2" t="n"/>
-      <c r="D25" s="2" t="n"/>
-      <c r="E25" s="2" t="n"/>
-      <c r="F25" s="2" t="inlineStr">
+      <c r="A25" s="4" t="n"/>
+      <c r="B25" s="4" t="n"/>
+      <c r="C25" s="4" t="n"/>
+      <c r="D25" s="4" t="n"/>
+      <c r="E25" s="4" t="n"/>
+      <c r="F25" s="4" t="inlineStr">
         <is>
           <t>Count: 4</t>
         </is>
       </c>
-      <c r="G25" s="2" t="n"/>
-      <c r="H25" s="2" t="inlineStr">
+      <c r="G25" s="4" t="n"/>
+      <c r="H25" s="4" t="inlineStr">
         <is>
           <t>16.50</t>
         </is>
       </c>
-      <c r="I25" s="2" t="inlineStr"/>
-      <c r="J25" s="2" t="n"/>
+      <c r="I25" s="4" t="n"/>
+      <c r="J25" s="4" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
+      <c r="A26" s="4" t="inlineStr">
         <is>
           <t>Employee: Buenrostro, Miranda</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="n"/>
+      <c r="A27" s="4" t="n"/>
       <c r="B27" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="n"/>
+      <c r="A28" s="4" t="n"/>
       <c r="B28" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="n"/>
+      <c r="A29" s="4" t="n"/>
       <c r="B29" s="3" t="n">
         <v>45574</v>
       </c>
@@ -1207,7 +1207,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="n"/>
+      <c r="A30" s="4" t="n"/>
       <c r="B30" s="3" t="n">
         <v>45575</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="n"/>
+      <c r="A31" s="4" t="n"/>
       <c r="B31" s="3" t="n">
         <v>45575</v>
       </c>
@@ -1268,34 +1268,34 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n"/>
-      <c r="B32" s="2" t="n"/>
-      <c r="C32" s="2" t="n"/>
-      <c r="D32" s="2" t="n"/>
-      <c r="E32" s="2" t="n"/>
-      <c r="F32" s="2" t="inlineStr">
+      <c r="A32" s="4" t="n"/>
+      <c r="B32" s="4" t="n"/>
+      <c r="C32" s="4" t="n"/>
+      <c r="D32" s="4" t="n"/>
+      <c r="E32" s="4" t="n"/>
+      <c r="F32" s="4" t="inlineStr">
         <is>
           <t>Count: 5</t>
         </is>
       </c>
-      <c r="G32" s="2" t="n"/>
-      <c r="H32" s="2" t="inlineStr">
+      <c r="G32" s="4" t="n"/>
+      <c r="H32" s="4" t="inlineStr">
         <is>
           <t>15.00</t>
         </is>
       </c>
-      <c r="I32" s="2" t="inlineStr"/>
-      <c r="J32" s="2" t="n"/>
+      <c r="I32" s="4" t="n"/>
+      <c r="J32" s="4" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="inlineStr">
+      <c r="A33" s="4" t="inlineStr">
         <is>
           <t>Employee: Contreras, Angel</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n"/>
+      <c r="A34" s="4" t="n"/>
       <c r="B34" s="3" t="n">
         <v>45571</v>
       </c>
@@ -1323,7 +1323,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n"/>
+      <c r="A35" s="4" t="n"/>
       <c r="B35" s="3" t="n">
         <v>45572</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="n"/>
+      <c r="A36" s="4" t="n"/>
       <c r="B36" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="n"/>
+      <c r="A37" s="4" t="n"/>
       <c r="B37" s="3" t="n">
         <v>45575</v>
       </c>
@@ -1417,34 +1417,34 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="n"/>
-      <c r="B38" s="2" t="n"/>
-      <c r="C38" s="2" t="n"/>
-      <c r="D38" s="2" t="n"/>
-      <c r="E38" s="2" t="n"/>
-      <c r="F38" s="2" t="inlineStr">
+      <c r="A38" s="4" t="n"/>
+      <c r="B38" s="4" t="n"/>
+      <c r="C38" s="4" t="n"/>
+      <c r="D38" s="4" t="n"/>
+      <c r="E38" s="4" t="n"/>
+      <c r="F38" s="4" t="inlineStr">
         <is>
           <t>Count: 4</t>
         </is>
       </c>
-      <c r="G38" s="2" t="n"/>
-      <c r="H38" s="2" t="inlineStr">
+      <c r="G38" s="4" t="n"/>
+      <c r="H38" s="4" t="inlineStr">
         <is>
           <t>13.00</t>
         </is>
       </c>
-      <c r="I38" s="2" t="inlineStr"/>
-      <c r="J38" s="2" t="n"/>
+      <c r="I38" s="4" t="n"/>
+      <c r="J38" s="4" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="inlineStr">
+      <c r="A39" s="4" t="inlineStr">
         <is>
           <t>Employee: Corcoran, Bradley (Brad)</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="n"/>
+      <c r="A40" s="4" t="n"/>
       <c r="B40" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1472,7 +1472,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n"/>
+      <c r="A41" s="4" t="n"/>
       <c r="B41" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1500,7 +1500,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n"/>
+      <c r="A42" s="4" t="n"/>
       <c r="B42" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1528,7 +1528,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="n"/>
+      <c r="A43" s="4" t="n"/>
       <c r="B43" s="3" t="n">
         <v>45575</v>
       </c>
@@ -1556,7 +1556,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="n"/>
+      <c r="A44" s="4" t="n"/>
       <c r="B44" s="3" t="n">
         <v>45575</v>
       </c>
@@ -1594,34 +1594,34 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="n"/>
-      <c r="B45" s="2" t="n"/>
-      <c r="C45" s="2" t="n"/>
-      <c r="D45" s="2" t="n"/>
-      <c r="E45" s="2" t="n"/>
-      <c r="F45" s="2" t="inlineStr">
+      <c r="A45" s="4" t="n"/>
+      <c r="B45" s="4" t="n"/>
+      <c r="C45" s="4" t="n"/>
+      <c r="D45" s="4" t="n"/>
+      <c r="E45" s="4" t="n"/>
+      <c r="F45" s="4" t="inlineStr">
         <is>
           <t>Count: 5</t>
         </is>
       </c>
-      <c r="G45" s="2" t="n"/>
-      <c r="H45" s="2" t="inlineStr">
+      <c r="G45" s="4" t="n"/>
+      <c r="H45" s="4" t="inlineStr">
         <is>
           <t>15.50</t>
         </is>
       </c>
-      <c r="I45" s="2" t="inlineStr"/>
-      <c r="J45" s="2" t="n"/>
+      <c r="I45" s="4" t="n"/>
+      <c r="J45" s="4" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="inlineStr">
+      <c r="A46" s="4" t="inlineStr">
         <is>
           <t>Employee: Dreyer, Eli</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="n"/>
+      <c r="A47" s="4" t="n"/>
       <c r="B47" s="3" t="n">
         <v>45572</v>
       </c>
@@ -1649,7 +1649,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="n"/>
+      <c r="A48" s="4" t="n"/>
       <c r="B48" s="3" t="n">
         <v>45574</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n"/>
+      <c r="A49" s="4" t="n"/>
       <c r="B49" s="3" t="n">
         <v>45574</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="n"/>
+      <c r="A50" s="4" t="n"/>
       <c r="B50" s="3" t="n">
         <v>45576</v>
       </c>
@@ -1743,34 +1743,34 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n"/>
-      <c r="B51" s="2" t="n"/>
-      <c r="C51" s="2" t="n"/>
-      <c r="D51" s="2" t="n"/>
-      <c r="E51" s="2" t="n"/>
-      <c r="F51" s="2" t="inlineStr">
+      <c r="A51" s="4" t="n"/>
+      <c r="B51" s="4" t="n"/>
+      <c r="C51" s="4" t="n"/>
+      <c r="D51" s="4" t="n"/>
+      <c r="E51" s="4" t="n"/>
+      <c r="F51" s="4" t="inlineStr">
         <is>
           <t>Count: 4</t>
         </is>
       </c>
-      <c r="G51" s="2" t="n"/>
-      <c r="H51" s="2" t="inlineStr">
+      <c r="G51" s="4" t="n"/>
+      <c r="H51" s="4" t="inlineStr">
         <is>
           <t>13.50</t>
         </is>
       </c>
-      <c r="I51" s="2" t="inlineStr"/>
-      <c r="J51" s="2" t="n"/>
+      <c r="I51" s="4" t="n"/>
+      <c r="J51" s="4" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="inlineStr">
+      <c r="A52" s="4" t="inlineStr">
         <is>
           <t>Employee: Fisher, Cole</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="n"/>
+      <c r="A53" s="4" t="n"/>
       <c r="B53" s="3" t="n">
         <v>45571</v>
       </c>
@@ -1798,7 +1798,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="n"/>
+      <c r="A54" s="4" t="n"/>
       <c r="B54" s="3" t="n">
         <v>45571</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="n"/>
+      <c r="A55" s="4" t="n"/>
       <c r="B55" s="3" t="n">
         <v>45575</v>
       </c>
@@ -1859,34 +1859,34 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="n"/>
-      <c r="B56" s="2" t="n"/>
-      <c r="C56" s="2" t="n"/>
-      <c r="D56" s="2" t="n"/>
-      <c r="E56" s="2" t="n"/>
-      <c r="F56" s="2" t="inlineStr">
+      <c r="A56" s="4" t="n"/>
+      <c r="B56" s="4" t="n"/>
+      <c r="C56" s="4" t="n"/>
+      <c r="D56" s="4" t="n"/>
+      <c r="E56" s="4" t="n"/>
+      <c r="F56" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G56" s="2" t="n"/>
-      <c r="H56" s="2" t="inlineStr">
+      <c r="G56" s="4" t="n"/>
+      <c r="H56" s="4" t="inlineStr">
         <is>
           <t>10.50</t>
         </is>
       </c>
-      <c r="I56" s="2" t="inlineStr"/>
-      <c r="J56" s="2" t="n"/>
+      <c r="I56" s="4" t="n"/>
+      <c r="J56" s="4" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="inlineStr">
+      <c r="A57" s="4" t="inlineStr">
         <is>
           <t>Employee: Fisher, Elisabeth</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="n"/>
+      <c r="A58" s="4" t="n"/>
       <c r="B58" s="3" t="n">
         <v>45572</v>
       </c>
@@ -1914,7 +1914,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="n"/>
+      <c r="A59" s="4" t="n"/>
       <c r="B59" s="3" t="n">
         <v>45573</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="n"/>
+      <c r="A60" s="4" t="n"/>
       <c r="B60" s="3" t="n">
         <v>45574</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="n"/>
+      <c r="A61" s="4" t="n"/>
       <c r="B61" s="3" t="n">
         <v>45576</v>
       </c>
@@ -2003,34 +2003,34 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n"/>
-      <c r="B62" s="2" t="n"/>
-      <c r="C62" s="2" t="n"/>
-      <c r="D62" s="2" t="n"/>
-      <c r="E62" s="2" t="n"/>
-      <c r="F62" s="2" t="inlineStr">
+      <c r="A62" s="4" t="n"/>
+      <c r="B62" s="4" t="n"/>
+      <c r="C62" s="4" t="n"/>
+      <c r="D62" s="4" t="n"/>
+      <c r="E62" s="4" t="n"/>
+      <c r="F62" s="4" t="inlineStr">
         <is>
           <t>Count: 4</t>
         </is>
       </c>
-      <c r="G62" s="2" t="n"/>
-      <c r="H62" s="2" t="inlineStr">
+      <c r="G62" s="4" t="n"/>
+      <c r="H62" s="4" t="inlineStr">
         <is>
           <t>13.50</t>
         </is>
       </c>
-      <c r="I62" s="2" t="inlineStr"/>
-      <c r="J62" s="2" t="n"/>
+      <c r="I62" s="4" t="n"/>
+      <c r="J62" s="4" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="inlineStr">
+      <c r="A63" s="4" t="inlineStr">
         <is>
           <t>Employee: Hayes, Charles</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="n"/>
+      <c r="A64" s="4" t="n"/>
       <c r="B64" s="3" t="n">
         <v>45571</v>
       </c>
@@ -2063,7 +2063,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="n"/>
+      <c r="A65" s="4" t="n"/>
       <c r="B65" s="3" t="n">
         <v>45573</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="n"/>
+      <c r="A66" s="4" t="n"/>
       <c r="B66" s="3" t="n">
         <v>45575</v>
       </c>
@@ -2129,34 +2129,34 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="n"/>
-      <c r="B67" s="2" t="n"/>
-      <c r="C67" s="2" t="n"/>
-      <c r="D67" s="2" t="n"/>
-      <c r="E67" s="2" t="n"/>
-      <c r="F67" s="2" t="inlineStr">
+      <c r="A67" s="4" t="n"/>
+      <c r="B67" s="4" t="n"/>
+      <c r="C67" s="4" t="n"/>
+      <c r="D67" s="4" t="n"/>
+      <c r="E67" s="4" t="n"/>
+      <c r="F67" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G67" s="2" t="n"/>
-      <c r="H67" s="2" t="inlineStr">
+      <c r="G67" s="4" t="n"/>
+      <c r="H67" s="4" t="inlineStr">
         <is>
           <t>9.00</t>
         </is>
       </c>
-      <c r="I67" s="2" t="inlineStr"/>
-      <c r="J67" s="2" t="n"/>
+      <c r="I67" s="4" t="n"/>
+      <c r="J67" s="4" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="inlineStr">
+      <c r="A68" s="4" t="inlineStr">
         <is>
           <t>Employee: Hendrickson, Stone</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="n"/>
+      <c r="A69" s="4" t="n"/>
       <c r="B69" s="3" t="n">
         <v>45572</v>
       </c>
@@ -2184,7 +2184,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="n"/>
+      <c r="A70" s="4" t="n"/>
       <c r="B70" s="3" t="n">
         <v>45572</v>
       </c>
@@ -2217,7 +2217,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="n"/>
+      <c r="A71" s="4" t="n"/>
       <c r="B71" s="3" t="n">
         <v>45573</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="n"/>
+      <c r="A72" s="4" t="n"/>
       <c r="B72" s="3" t="n">
         <v>45574</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="n"/>
+      <c r="A73" s="4" t="n"/>
       <c r="B73" s="3" t="n">
         <v>45575</v>
       </c>
@@ -2311,7 +2311,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="n"/>
+      <c r="A74" s="4" t="n"/>
       <c r="B74" s="3" t="n">
         <v>45576</v>
       </c>
@@ -2339,34 +2339,34 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="n"/>
-      <c r="B75" s="2" t="n"/>
-      <c r="C75" s="2" t="n"/>
-      <c r="D75" s="2" t="n"/>
-      <c r="E75" s="2" t="n"/>
-      <c r="F75" s="2" t="inlineStr">
+      <c r="A75" s="4" t="n"/>
+      <c r="B75" s="4" t="n"/>
+      <c r="C75" s="4" t="n"/>
+      <c r="D75" s="4" t="n"/>
+      <c r="E75" s="4" t="n"/>
+      <c r="F75" s="4" t="inlineStr">
         <is>
           <t>Count: 6</t>
         </is>
       </c>
-      <c r="G75" s="2" t="n"/>
-      <c r="H75" s="2" t="inlineStr">
+      <c r="G75" s="4" t="n"/>
+      <c r="H75" s="4" t="inlineStr">
         <is>
           <t>19.50</t>
         </is>
       </c>
-      <c r="I75" s="2" t="inlineStr"/>
-      <c r="J75" s="2" t="n"/>
+      <c r="I75" s="4" t="n"/>
+      <c r="J75" s="4" t="n"/>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="inlineStr">
+      <c r="A76" s="4" t="inlineStr">
         <is>
           <t>Employee: Holmes, Alexander (Alex)</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="n"/>
+      <c r="A77" s="4" t="n"/>
       <c r="B77" s="3" t="n">
         <v>45571</v>
       </c>
@@ -2394,7 +2394,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="n"/>
+      <c r="A78" s="4" t="n"/>
       <c r="B78" s="3" t="n">
         <v>45572</v>
       </c>
@@ -2432,7 +2432,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="n"/>
+      <c r="A79" s="4" t="n"/>
       <c r="B79" s="3" t="n">
         <v>45575</v>
       </c>
@@ -2465,7 +2465,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="n"/>
+      <c r="A80" s="4" t="n"/>
       <c r="B80" s="3" t="n">
         <v>45575</v>
       </c>
@@ -2498,34 +2498,34 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="n"/>
-      <c r="B81" s="2" t="n"/>
-      <c r="C81" s="2" t="n"/>
-      <c r="D81" s="2" t="n"/>
-      <c r="E81" s="2" t="n"/>
-      <c r="F81" s="2" t="inlineStr">
+      <c r="A81" s="4" t="n"/>
+      <c r="B81" s="4" t="n"/>
+      <c r="C81" s="4" t="n"/>
+      <c r="D81" s="4" t="n"/>
+      <c r="E81" s="4" t="n"/>
+      <c r="F81" s="4" t="inlineStr">
         <is>
           <t>Count: 4</t>
         </is>
       </c>
-      <c r="G81" s="2" t="n"/>
-      <c r="H81" s="2" t="inlineStr">
+      <c r="G81" s="4" t="n"/>
+      <c r="H81" s="4" t="inlineStr">
         <is>
           <t>16.50</t>
         </is>
       </c>
-      <c r="I81" s="2" t="inlineStr"/>
-      <c r="J81" s="2" t="n"/>
+      <c r="I81" s="4" t="n"/>
+      <c r="J81" s="4" t="n"/>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="inlineStr">
+      <c r="A82" s="4" t="inlineStr">
         <is>
           <t>Employee: Jaeckel, Jessica</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="n"/>
+      <c r="A83" s="4" t="n"/>
       <c r="B83" s="3" t="n">
         <v>45572</v>
       </c>
@@ -2553,7 +2553,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="n"/>
+      <c r="A84" s="4" t="n"/>
       <c r="B84" s="3" t="n">
         <v>45573</v>
       </c>
@@ -2581,7 +2581,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="n"/>
+      <c r="A85" s="4" t="n"/>
       <c r="B85" s="3" t="n">
         <v>45574</v>
       </c>
@@ -2619,34 +2619,34 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="n"/>
-      <c r="B86" s="2" t="n"/>
-      <c r="C86" s="2" t="n"/>
-      <c r="D86" s="2" t="n"/>
-      <c r="E86" s="2" t="n"/>
-      <c r="F86" s="2" t="inlineStr">
+      <c r="A86" s="4" t="n"/>
+      <c r="B86" s="4" t="n"/>
+      <c r="C86" s="4" t="n"/>
+      <c r="D86" s="4" t="n"/>
+      <c r="E86" s="4" t="n"/>
+      <c r="F86" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G86" s="2" t="n"/>
-      <c r="H86" s="2" t="inlineStr">
+      <c r="G86" s="4" t="n"/>
+      <c r="H86" s="4" t="inlineStr">
         <is>
           <t>10.50</t>
         </is>
       </c>
-      <c r="I86" s="2" t="inlineStr"/>
-      <c r="J86" s="2" t="n"/>
+      <c r="I86" s="4" t="n"/>
+      <c r="J86" s="4" t="n"/>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="inlineStr">
+      <c r="A87" s="4" t="inlineStr">
         <is>
           <t>Employee: Jorgensen, Samuel</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="n"/>
+      <c r="A88" s="4" t="n"/>
       <c r="B88" s="3" t="n">
         <v>45571</v>
       </c>
@@ -2674,7 +2674,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="n"/>
+      <c r="A89" s="4" t="n"/>
       <c r="B89" s="3" t="n">
         <v>45572</v>
       </c>
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="n"/>
+      <c r="A90" s="4" t="n"/>
       <c r="B90" s="3" t="n">
         <v>45575</v>
       </c>
@@ -2735,34 +2735,34 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="n"/>
-      <c r="B91" s="2" t="n"/>
-      <c r="C91" s="2" t="n"/>
-      <c r="D91" s="2" t="n"/>
-      <c r="E91" s="2" t="n"/>
-      <c r="F91" s="2" t="inlineStr">
+      <c r="A91" s="4" t="n"/>
+      <c r="B91" s="4" t="n"/>
+      <c r="C91" s="4" t="n"/>
+      <c r="D91" s="4" t="n"/>
+      <c r="E91" s="4" t="n"/>
+      <c r="F91" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G91" s="2" t="n"/>
-      <c r="H91" s="2" t="inlineStr">
+      <c r="G91" s="4" t="n"/>
+      <c r="H91" s="4" t="inlineStr">
         <is>
           <t>10.50</t>
         </is>
       </c>
-      <c r="I91" s="2" t="inlineStr"/>
-      <c r="J91" s="2" t="n"/>
+      <c r="I91" s="4" t="n"/>
+      <c r="J91" s="4" t="n"/>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="inlineStr">
+      <c r="A92" s="4" t="inlineStr">
         <is>
           <t>Employee: Kundu, Dipro</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n"/>
+      <c r="A93" s="4" t="n"/>
       <c r="B93" s="3" t="n">
         <v>45571</v>
       </c>
@@ -2790,7 +2790,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="n"/>
+      <c r="A94" s="4" t="n"/>
       <c r="B94" s="3" t="n">
         <v>45571</v>
       </c>
@@ -2818,7 +2818,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="n"/>
+      <c r="A95" s="4" t="n"/>
       <c r="B95" s="3" t="n">
         <v>45574</v>
       </c>
@@ -2846,7 +2846,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="n"/>
+      <c r="A96" s="4" t="n"/>
       <c r="B96" s="3" t="n">
         <v>45574</v>
       </c>
@@ -2879,7 +2879,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="n"/>
+      <c r="A97" s="4" t="n"/>
       <c r="B97" s="3" t="n">
         <v>45576</v>
       </c>
@@ -2912,34 +2912,34 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="n"/>
-      <c r="B98" s="2" t="n"/>
-      <c r="C98" s="2" t="n"/>
-      <c r="D98" s="2" t="n"/>
-      <c r="E98" s="2" t="n"/>
-      <c r="F98" s="2" t="inlineStr">
+      <c r="A98" s="4" t="n"/>
+      <c r="B98" s="4" t="n"/>
+      <c r="C98" s="4" t="n"/>
+      <c r="D98" s="4" t="n"/>
+      <c r="E98" s="4" t="n"/>
+      <c r="F98" s="4" t="inlineStr">
         <is>
           <t>Count: 5</t>
         </is>
       </c>
-      <c r="G98" s="2" t="n"/>
-      <c r="H98" s="2" t="inlineStr">
+      <c r="G98" s="4" t="n"/>
+      <c r="H98" s="4" t="inlineStr">
         <is>
           <t>18.00</t>
         </is>
       </c>
-      <c r="I98" s="2" t="inlineStr"/>
-      <c r="J98" s="2" t="n"/>
+      <c r="I98" s="4" t="n"/>
+      <c r="J98" s="4" t="n"/>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="inlineStr">
+      <c r="A99" s="4" t="inlineStr">
         <is>
           <t>Employee: Le, Minh</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="n"/>
+      <c r="A100" s="4" t="n"/>
       <c r="B100" s="3" t="n">
         <v>45572</v>
       </c>
@@ -2972,7 +2972,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="n"/>
+      <c r="A101" s="4" t="n"/>
       <c r="B101" s="3" t="n">
         <v>45572</v>
       </c>
@@ -3005,7 +3005,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="n"/>
+      <c r="A102" s="4" t="n"/>
       <c r="B102" s="3" t="n">
         <v>45574</v>
       </c>
@@ -3033,7 +3033,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="n"/>
+      <c r="A103" s="4" t="n"/>
       <c r="B103" s="3" t="n">
         <v>45574</v>
       </c>
@@ -3061,7 +3061,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="n"/>
+      <c r="A104" s="4" t="n"/>
       <c r="B104" s="3" t="n">
         <v>45576</v>
       </c>
@@ -3089,34 +3089,34 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="n"/>
-      <c r="B105" s="2" t="n"/>
-      <c r="C105" s="2" t="n"/>
-      <c r="D105" s="2" t="n"/>
-      <c r="E105" s="2" t="n"/>
-      <c r="F105" s="2" t="inlineStr">
+      <c r="A105" s="4" t="n"/>
+      <c r="B105" s="4" t="n"/>
+      <c r="C105" s="4" t="n"/>
+      <c r="D105" s="4" t="n"/>
+      <c r="E105" s="4" t="n"/>
+      <c r="F105" s="4" t="inlineStr">
         <is>
           <t>Count: 5</t>
         </is>
       </c>
-      <c r="G105" s="2" t="n"/>
-      <c r="H105" s="2" t="inlineStr">
+      <c r="G105" s="4" t="n"/>
+      <c r="H105" s="4" t="inlineStr">
         <is>
           <t>16.00</t>
         </is>
       </c>
-      <c r="I105" s="2" t="inlineStr"/>
-      <c r="J105" s="2" t="n"/>
+      <c r="I105" s="4" t="n"/>
+      <c r="J105" s="4" t="n"/>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="inlineStr">
+      <c r="A106" s="4" t="inlineStr">
         <is>
           <t>Employee: Mahendran, Kishorre</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="n"/>
+      <c r="A107" s="4" t="n"/>
       <c r="B107" s="3" t="n">
         <v>45571</v>
       </c>
@@ -3144,7 +3144,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="n"/>
+      <c r="A108" s="4" t="n"/>
       <c r="B108" s="3" t="n">
         <v>45572</v>
       </c>
@@ -3182,7 +3182,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="n"/>
+      <c r="A109" s="4" t="n"/>
       <c r="B109" s="3" t="n">
         <v>45576</v>
       </c>
@@ -3210,34 +3210,34 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="n"/>
-      <c r="B110" s="2" t="n"/>
-      <c r="C110" s="2" t="n"/>
-      <c r="D110" s="2" t="n"/>
-      <c r="E110" s="2" t="n"/>
-      <c r="F110" s="2" t="inlineStr">
+      <c r="A110" s="4" t="n"/>
+      <c r="B110" s="4" t="n"/>
+      <c r="C110" s="4" t="n"/>
+      <c r="D110" s="4" t="n"/>
+      <c r="E110" s="4" t="n"/>
+      <c r="F110" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G110" s="2" t="n"/>
-      <c r="H110" s="2" t="inlineStr">
+      <c r="G110" s="4" t="n"/>
+      <c r="H110" s="4" t="inlineStr">
         <is>
           <t>10.00</t>
         </is>
       </c>
-      <c r="I110" s="2" t="inlineStr"/>
-      <c r="J110" s="2" t="n"/>
+      <c r="I110" s="4" t="n"/>
+      <c r="J110" s="4" t="n"/>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="inlineStr">
+      <c r="A111" s="4" t="inlineStr">
         <is>
           <t>Employee: Murphy, Kelton</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="n"/>
+      <c r="A112" s="4" t="n"/>
       <c r="B112" s="3" t="n">
         <v>45572</v>
       </c>
@@ -3265,7 +3265,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="n"/>
+      <c r="A113" s="4" t="n"/>
       <c r="B113" s="3" t="n">
         <v>45573</v>
       </c>
@@ -3298,7 +3298,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="n"/>
+      <c r="A114" s="4" t="n"/>
       <c r="B114" s="3" t="n">
         <v>45574</v>
       </c>
@@ -3326,7 +3326,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="n"/>
+      <c r="A115" s="4" t="n"/>
       <c r="B115" s="3" t="n">
         <v>45576</v>
       </c>
@@ -3354,34 +3354,34 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="n"/>
-      <c r="B116" s="2" t="n"/>
-      <c r="C116" s="2" t="n"/>
-      <c r="D116" s="2" t="n"/>
-      <c r="E116" s="2" t="n"/>
-      <c r="F116" s="2" t="inlineStr">
+      <c r="A116" s="4" t="n"/>
+      <c r="B116" s="4" t="n"/>
+      <c r="C116" s="4" t="n"/>
+      <c r="D116" s="4" t="n"/>
+      <c r="E116" s="4" t="n"/>
+      <c r="F116" s="4" t="inlineStr">
         <is>
           <t>Count: 4</t>
         </is>
       </c>
-      <c r="G116" s="2" t="n"/>
-      <c r="H116" s="2" t="inlineStr">
+      <c r="G116" s="4" t="n"/>
+      <c r="H116" s="4" t="inlineStr">
         <is>
           <t>12.50</t>
         </is>
       </c>
-      <c r="I116" s="2" t="inlineStr"/>
-      <c r="J116" s="2" t="n"/>
+      <c r="I116" s="4" t="n"/>
+      <c r="J116" s="4" t="n"/>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="inlineStr">
+      <c r="A117" s="4" t="inlineStr">
         <is>
           <t>Employee: Perez Munoz, Leonardo</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="n"/>
+      <c r="A118" s="4" t="n"/>
       <c r="B118" s="3" t="n">
         <v>45571</v>
       </c>
@@ -3409,7 +3409,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="n"/>
+      <c r="A119" s="4" t="n"/>
       <c r="B119" s="3" t="n">
         <v>45572</v>
       </c>
@@ -3437,7 +3437,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="n"/>
+      <c r="A120" s="4" t="n"/>
       <c r="B120" s="3" t="n">
         <v>45573</v>
       </c>
@@ -3475,34 +3475,34 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="n"/>
-      <c r="B121" s="2" t="n"/>
-      <c r="C121" s="2" t="n"/>
-      <c r="D121" s="2" t="n"/>
-      <c r="E121" s="2" t="n"/>
-      <c r="F121" s="2" t="inlineStr">
+      <c r="A121" s="4" t="n"/>
+      <c r="B121" s="4" t="n"/>
+      <c r="C121" s="4" t="n"/>
+      <c r="D121" s="4" t="n"/>
+      <c r="E121" s="4" t="n"/>
+      <c r="F121" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G121" s="2" t="n"/>
-      <c r="H121" s="2" t="inlineStr">
+      <c r="G121" s="4" t="n"/>
+      <c r="H121" s="4" t="inlineStr">
         <is>
           <t>10.50</t>
         </is>
       </c>
-      <c r="I121" s="2" t="inlineStr"/>
-      <c r="J121" s="2" t="n"/>
+      <c r="I121" s="4" t="n"/>
+      <c r="J121" s="4" t="n"/>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="inlineStr">
+      <c r="A122" s="4" t="inlineStr">
         <is>
           <t>Employee: Schiltz, Margaret (Maggie)</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="n"/>
+      <c r="A123" s="4" t="n"/>
       <c r="B123" s="3" t="n">
         <v>45572</v>
       </c>
@@ -3530,7 +3530,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="2" t="n"/>
+      <c r="A124" s="4" t="n"/>
       <c r="B124" s="3" t="n">
         <v>45574</v>
       </c>
@@ -3563,7 +3563,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="2" t="n"/>
+      <c r="A125" s="4" t="n"/>
       <c r="B125" s="3" t="n">
         <v>45576</v>
       </c>
@@ -3591,34 +3591,34 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="2" t="n"/>
-      <c r="B126" s="2" t="n"/>
-      <c r="C126" s="2" t="n"/>
-      <c r="D126" s="2" t="n"/>
-      <c r="E126" s="2" t="n"/>
-      <c r="F126" s="2" t="inlineStr">
+      <c r="A126" s="4" t="n"/>
+      <c r="B126" s="4" t="n"/>
+      <c r="C126" s="4" t="n"/>
+      <c r="D126" s="4" t="n"/>
+      <c r="E126" s="4" t="n"/>
+      <c r="F126" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G126" s="2" t="n"/>
-      <c r="H126" s="2" t="inlineStr">
+      <c r="G126" s="4" t="n"/>
+      <c r="H126" s="4" t="inlineStr">
         <is>
           <t>11.00</t>
         </is>
       </c>
-      <c r="I126" s="2" t="inlineStr"/>
-      <c r="J126" s="2" t="n"/>
+      <c r="I126" s="4" t="n"/>
+      <c r="J126" s="4" t="n"/>
     </row>
     <row r="127">
-      <c r="A127" s="2" t="inlineStr">
+      <c r="A127" s="4" t="inlineStr">
         <is>
           <t>Employee: Szewczyk, Jacob</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="n"/>
+      <c r="A128" s="4" t="n"/>
       <c r="B128" s="3" t="n">
         <v>45571</v>
       </c>
@@ -3646,7 +3646,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="n"/>
+      <c r="A129" s="4" t="n"/>
       <c r="B129" s="3" t="n">
         <v>45571</v>
       </c>
@@ -3674,34 +3674,34 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="n"/>
-      <c r="B130" s="2" t="n"/>
-      <c r="C130" s="2" t="n"/>
-      <c r="D130" s="2" t="n"/>
-      <c r="E130" s="2" t="n"/>
-      <c r="F130" s="2" t="inlineStr">
+      <c r="A130" s="4" t="n"/>
+      <c r="B130" s="4" t="n"/>
+      <c r="C130" s="4" t="n"/>
+      <c r="D130" s="4" t="n"/>
+      <c r="E130" s="4" t="n"/>
+      <c r="F130" s="4" t="inlineStr">
         <is>
           <t>Count: 2</t>
         </is>
       </c>
-      <c r="G130" s="2" t="n"/>
-      <c r="H130" s="2" t="inlineStr">
+      <c r="G130" s="4" t="n"/>
+      <c r="H130" s="4" t="inlineStr">
         <is>
           <t>7.50</t>
         </is>
       </c>
-      <c r="I130" s="2" t="inlineStr"/>
-      <c r="J130" s="2" t="n"/>
+      <c r="I130" s="4" t="n"/>
+      <c r="J130" s="4" t="n"/>
     </row>
     <row r="131">
-      <c r="A131" s="2" t="inlineStr">
+      <c r="A131" s="4" t="inlineStr">
         <is>
           <t>Employee: Taege, Caden</t>
         </is>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="2" t="n"/>
+      <c r="A132" s="4" t="n"/>
       <c r="B132" s="3" t="n">
         <v>45571</v>
       </c>
@@ -3734,7 +3734,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="2" t="n"/>
+      <c r="A133" s="4" t="n"/>
       <c r="B133" s="3" t="n">
         <v>45571</v>
       </c>
@@ -3767,7 +3767,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="2" t="n"/>
+      <c r="A134" s="4" t="n"/>
       <c r="B134" s="3" t="n">
         <v>45572</v>
       </c>
@@ -3800,34 +3800,34 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="2" t="n"/>
-      <c r="B135" s="2" t="n"/>
-      <c r="C135" s="2" t="n"/>
-      <c r="D135" s="2" t="n"/>
-      <c r="E135" s="2" t="n"/>
-      <c r="F135" s="2" t="inlineStr">
+      <c r="A135" s="4" t="n"/>
+      <c r="B135" s="4" t="n"/>
+      <c r="C135" s="4" t="n"/>
+      <c r="D135" s="4" t="n"/>
+      <c r="E135" s="4" t="n"/>
+      <c r="F135" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G135" s="2" t="n"/>
-      <c r="H135" s="2" t="inlineStr">
+      <c r="G135" s="4" t="n"/>
+      <c r="H135" s="4" t="inlineStr">
         <is>
           <t>10.50</t>
         </is>
       </c>
-      <c r="I135" s="2" t="inlineStr"/>
-      <c r="J135" s="2" t="n"/>
+      <c r="I135" s="4" t="n"/>
+      <c r="J135" s="4" t="n"/>
     </row>
     <row r="136">
-      <c r="A136" s="2" t="inlineStr">
+      <c r="A136" s="4" t="inlineStr">
         <is>
           <t>Employee: Willis, Ava</t>
         </is>
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="2" t="n"/>
+      <c r="A137" s="4" t="n"/>
       <c r="B137" s="3" t="n">
         <v>45572</v>
       </c>
@@ -3860,7 +3860,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="2" t="n"/>
+      <c r="A138" s="4" t="n"/>
       <c r="B138" s="3" t="n">
         <v>45574</v>
       </c>
@@ -3888,7 +3888,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="2" t="n"/>
+      <c r="A139" s="4" t="n"/>
       <c r="B139" s="3" t="n">
         <v>45576</v>
       </c>
@@ -3916,44 +3916,44 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="n"/>
-      <c r="B140" s="2" t="n"/>
-      <c r="C140" s="2" t="n"/>
-      <c r="D140" s="2" t="n"/>
-      <c r="E140" s="2" t="n"/>
-      <c r="F140" s="2" t="inlineStr">
+      <c r="A140" s="4" t="n"/>
+      <c r="B140" s="4" t="n"/>
+      <c r="C140" s="4" t="n"/>
+      <c r="D140" s="4" t="n"/>
+      <c r="E140" s="4" t="n"/>
+      <c r="F140" s="4" t="inlineStr">
         <is>
           <t>Count: 3</t>
         </is>
       </c>
-      <c r="G140" s="2" t="n"/>
-      <c r="H140" s="2" t="inlineStr">
+      <c r="G140" s="4" t="n"/>
+      <c r="H140" s="4" t="inlineStr">
         <is>
           <t>9.50</t>
         </is>
       </c>
-      <c r="I140" s="2" t="inlineStr"/>
-      <c r="J140" s="2" t="n"/>
+      <c r="I140" s="4" t="n"/>
+      <c r="J140" s="4" t="n"/>
     </row>
     <row r="141">
-      <c r="A141" s="2" t="n"/>
-      <c r="B141" s="2" t="n"/>
-      <c r="C141" s="2" t="n"/>
-      <c r="D141" s="2" t="n"/>
-      <c r="E141" s="2" t="n"/>
-      <c r="F141" s="2" t="inlineStr">
+      <c r="A141" s="4" t="n"/>
+      <c r="B141" s="4" t="n"/>
+      <c r="C141" s="4" t="n"/>
+      <c r="D141" s="4" t="n"/>
+      <c r="E141" s="4" t="n"/>
+      <c r="F141" s="4" t="inlineStr">
         <is>
           <t>Count: 91</t>
         </is>
       </c>
-      <c r="G141" s="2" t="n"/>
-      <c r="H141" s="2" t="inlineStr">
+      <c r="G141" s="4" t="n"/>
+      <c r="H141" s="4" t="inlineStr">
         <is>
           <t>310.50</t>
         </is>
       </c>
-      <c r="I141" s="2" t="inlineStr"/>
-      <c r="J141" s="2" t="n"/>
+      <c r="I141" s="4" t="n"/>
+      <c r="J141" s="4" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -3998,7 +3998,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">

</xml_diff>